<commit_message>
admin page and user data upd
</commit_message>
<xml_diff>
--- a/BillAppDocs/UsersUploadData.xlsx
+++ b/BillAppDocs/UsersUploadData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyDir\Walee\Bill-Website-Walee\BillAppDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BECDA51-41BF-4262-83B5-6A7BF40DFA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BD35F3-D1A5-4047-9CD8-43BE8C667CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <t>Ali</t>
   </si>
   <si>
-    <t>H-12 Sector</t>
+    <t>H-12 Sector, ISB</t>
   </si>
 </sst>
 </file>

</xml_diff>